<commit_message>
complete the RELAY_TEST_V10A project.
</commit_message>
<xml_diff>
--- a/RELAY_TEST_V10A/SCH/RELAY_TEST_V10A_继电器定时开关_V1.0.xlsx
+++ b/RELAY_TEST_V10A/SCH/RELAY_TEST_V10A_继电器定时开关_V1.0.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="211">
   <si>
     <t>设计</t>
   </si>
@@ -87,13 +87,589 @@
   <si>
     <t>1、</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>BEEP</t>
+  </si>
+  <si>
+    <t>BEEP_12X7R6</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>330uF_50V_10X13</t>
+  </si>
+  <si>
+    <t>CAP-5R0-10X13</t>
+  </si>
+  <si>
+    <t>Cap,50V,10x13,ESK337M1HG13RR</t>
+  </si>
+  <si>
+    <t>SAMXON</t>
+  </si>
+  <si>
+    <t>C2,C4,C7,C12,C13,C14,C15,</t>
+  </si>
+  <si>
+    <t>0.1uF_50V</t>
+  </si>
+  <si>
+    <t>CC0603</t>
+  </si>
+  <si>
+    <t>CAP,CERM,+/-10%,X7R,0603</t>
+  </si>
+  <si>
+    <t>FH</t>
+  </si>
+  <si>
+    <t>C16,C18,C19,C20,C21,C22,</t>
+  </si>
+  <si>
+    <t>C23,C24,C25,C26</t>
+  </si>
+  <si>
+    <t>10uF_25V</t>
+  </si>
+  <si>
+    <t>CC0805</t>
+  </si>
+  <si>
+    <t>CAP,CERM,+/-10%,X5R,0805</t>
+  </si>
+  <si>
+    <t>C5,C6,C17</t>
+  </si>
+  <si>
+    <t>12pF_50V</t>
+  </si>
+  <si>
+    <t>CAP,CERM,+/-10%,C0G,0603</t>
+  </si>
+  <si>
+    <t>20pF_50V</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>22uF_25V_3528</t>
+  </si>
+  <si>
+    <t>CC3528_12</t>
+  </si>
+  <si>
+    <t>CAP,TAN,TAJB226K025RNJ</t>
+  </si>
+  <si>
+    <t>AVX</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>47uF_10V_3528</t>
+  </si>
+  <si>
+    <t>CAP,TAN,TAJB476K010RNJ</t>
+  </si>
+  <si>
+    <t>D1,D2,D3</t>
+  </si>
+  <si>
+    <t>1N4148W-TP</t>
+  </si>
+  <si>
+    <t>SOD-123</t>
+  </si>
+  <si>
+    <t>High Speed Switching Diode 400mW</t>
+  </si>
+  <si>
+    <t>MCC</t>
+  </si>
+  <si>
+    <t>D4,D5,D6</t>
+  </si>
+  <si>
+    <t>LED_RED</t>
+  </si>
+  <si>
+    <t>led0805</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>FUSE_3.15A_25VAC</t>
+  </si>
+  <si>
+    <t>FUSE_D5</t>
+  </si>
+  <si>
+    <t>FUSE,250V AC,2A</t>
+  </si>
+  <si>
+    <t>AEM</t>
+  </si>
+  <si>
+    <t>J1,J2</t>
+  </si>
+  <si>
+    <t>KF7R62-2P</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>ARL2F-P</t>
+  </si>
+  <si>
+    <t>RELAY</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>HEADER3X2_2R54</t>
+  </si>
+  <si>
+    <t>Nextron</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>XH-6A</t>
+  </si>
+  <si>
+    <t>L1,L2,L3,L4</t>
+  </si>
+  <si>
+    <t>BEAD_BLM21PG600</t>
+  </si>
+  <si>
+    <t>LC0805</t>
+  </si>
+  <si>
+    <t>BEAD,60R/100MHz,6A,0805</t>
+  </si>
+  <si>
+    <t>muRata</t>
+  </si>
+  <si>
+    <t>MH1,MH2,MH3,MH4</t>
+  </si>
+  <si>
+    <t>Hold-M3</t>
+  </si>
+  <si>
+    <t>HOLD250D134</t>
+  </si>
+  <si>
+    <t>Hold</t>
+  </si>
+  <si>
+    <t>MP1,MP2</t>
+  </si>
+  <si>
+    <t>MarkPoint</t>
+  </si>
+  <si>
+    <t>MARKPOINT_R3</t>
+  </si>
+  <si>
+    <t>MARK POINT</t>
+  </si>
+  <si>
+    <t>OP1</t>
+  </si>
+  <si>
+    <t>TLP127</t>
+  </si>
+  <si>
+    <t>SO-1346</t>
+  </si>
+  <si>
+    <t>GaAs Ired &amp; Photo Transistor</t>
+  </si>
+  <si>
+    <t>TOSHIBA</t>
+  </si>
+  <si>
+    <t>Q1,Q4</t>
+  </si>
+  <si>
+    <t>S8050_NPN</t>
+  </si>
+  <si>
+    <t>SOT23_123</t>
+  </si>
+  <si>
+    <t>SOT-23 Plastic-Encapsulate Transistors</t>
+  </si>
+  <si>
+    <t>CJ</t>
+  </si>
+  <si>
+    <t>Q2,Q3</t>
+  </si>
+  <si>
+    <t>BCV47_NPN</t>
+  </si>
+  <si>
+    <t>Transistor,NPN,45V,0.5A,SOT23-3</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>S8550_PNP</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>S8050_SOT23_NPN</t>
+  </si>
+  <si>
+    <t>R1,R2,R3,R10,R22,R23,R26,</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>RC0603</t>
+  </si>
+  <si>
+    <t>RES,1%,0.1W,0603</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>R5,R6,R7,R11</t>
+  </si>
+  <si>
+    <t>10R</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>20K</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>100R</t>
+  </si>
+  <si>
+    <t>R17,R21,R24,R25</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>R18,R37</t>
+  </si>
+  <si>
+    <t>0R/NI</t>
+  </si>
+  <si>
+    <t>R19,R20,R31,R35,R36</t>
+  </si>
+  <si>
+    <t>4.7K</t>
+  </si>
+  <si>
+    <t>R28,R32,R34</t>
+  </si>
+  <si>
+    <t>510R</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>R39</t>
+  </si>
+  <si>
+    <t>47K</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>SWITCH_3P</t>
+  </si>
+  <si>
+    <t>SW2,SW3,SW4,SW5</t>
+  </si>
+  <si>
+    <t>SWITCH</t>
+  </si>
+  <si>
+    <t>SW-6X6x6-L</t>
+  </si>
+  <si>
+    <t>USB1</t>
+  </si>
+  <si>
+    <t>USB-MICRO</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>STM32F103RxT6</t>
+  </si>
+  <si>
+    <t>LQFP-64</t>
+  </si>
+  <si>
+    <t>ST Cortex-m3 MCU</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>TFT-2R4</t>
+  </si>
+  <si>
+    <t>ILI9341 2.4 TFT</t>
+  </si>
+  <si>
+    <t>ILI</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>HLK-PM12</t>
+  </si>
+  <si>
+    <t>ACDC MODULA</t>
+  </si>
+  <si>
+    <t>HI-LINK</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>XPT2046</t>
+  </si>
+  <si>
+    <t>TSSOP-16</t>
+  </si>
+  <si>
+    <t>Touch Screen Controller</t>
+  </si>
+  <si>
+    <t>XPT</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>HPSD1233I2A</t>
+  </si>
+  <si>
+    <t>PTH05000WAH</t>
+  </si>
+  <si>
+    <t>DCDC MODULAR</t>
+  </si>
+  <si>
+    <t>HYOC</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>BATTERY_CR1220</t>
+  </si>
+  <si>
+    <t>CR1220</t>
+  </si>
+  <si>
+    <t>CR1220 HOLD</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>AT24C512C-SSHM-T</t>
+  </si>
+  <si>
+    <t>SOIC8</t>
+  </si>
+  <si>
+    <t>IIC Serial EEPROM 512Kbit</t>
+  </si>
+  <si>
+    <t>ATMEL</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>PCF8563</t>
+  </si>
+  <si>
+    <t>RTC</t>
+  </si>
+  <si>
+    <t>NXP</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>W25Q128FVSIG</t>
+  </si>
+  <si>
+    <t>SOIC-8_208</t>
+  </si>
+  <si>
+    <t>3V 128M-BIT SPI FLASH</t>
+  </si>
+  <si>
+    <t>WINBOND</t>
+  </si>
+  <si>
+    <t>U10</t>
+  </si>
+  <si>
+    <t>CH340G</t>
+  </si>
+  <si>
+    <t>SOIC16</t>
+  </si>
+  <si>
+    <t>USB to UART</t>
+  </si>
+  <si>
+    <t>WCH</t>
+  </si>
+  <si>
+    <t>U11</t>
+  </si>
+  <si>
+    <t>TFCARD</t>
+  </si>
+  <si>
+    <t>TFCARD HOLD</t>
+  </si>
+  <si>
+    <t>U22</t>
+  </si>
+  <si>
+    <t>AMS1117-3.3</t>
+  </si>
+  <si>
+    <t>SOT-223</t>
+  </si>
+  <si>
+    <t>1A LOW DROPOUT VOLTAGE REGULATOR</t>
+  </si>
+  <si>
+    <t>AMS</t>
+  </si>
+  <si>
+    <t>VSR1</t>
+  </si>
+  <si>
+    <t>14D471K</t>
+  </si>
+  <si>
+    <t>14D220K</t>
+  </si>
+  <si>
+    <t>VARISTOR</t>
+  </si>
+  <si>
+    <t>X1,X3</t>
+  </si>
+  <si>
+    <t>XTAL_32768Hz_3215</t>
+  </si>
+  <si>
+    <t>X-2P-3R2X1R5-SMD</t>
+  </si>
+  <si>
+    <t>Q13FC1350000400</t>
+  </si>
+  <si>
+    <t>EPSON</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>XTAL_8MHz_5032</t>
+  </si>
+  <si>
+    <t>X-2P-5R0X3R2-SMD</t>
+  </si>
+  <si>
+    <t>X50328MSD2GC</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>XTAL_12MHz_5032</t>
+  </si>
+  <si>
+    <t>X503212MSD2GC</t>
+  </si>
+  <si>
+    <t>C3,C85,C86,C89,C90</t>
+  </si>
+  <si>
+    <t>C8,C9,C27,C28</t>
+  </si>
+  <si>
+    <t>R8,R12,R13,R27,R30,R33,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -152,16 +728,42 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -247,11 +849,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -276,6 +895,12 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -322,9 +947,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="差" xfId="2" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -599,9 +1241,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:I35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -619,97 +1261,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="23"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="11" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18"/>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11" t="s">
+      <c r="A3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="11" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
@@ -743,665 +1385,1409 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
+      <c r="A8" s="10">
+        <v>1</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
+      <c r="A9" s="10">
+        <v>2</v>
+      </c>
+      <c r="B9" s="10">
+        <v>1</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
+      <c r="A10" s="26">
+        <v>3</v>
+      </c>
+      <c r="B10" s="26">
+        <v>17</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
+      <c r="A13" s="10">
+        <v>4</v>
+      </c>
+      <c r="B13" s="10">
+        <v>5</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
+      <c r="A14" s="10">
+        <v>5</v>
+      </c>
+      <c r="B14" s="10">
+        <v>3</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
+      <c r="A15" s="10">
+        <v>6</v>
+      </c>
+      <c r="B15" s="10">
+        <v>4</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
+      <c r="A16" s="10">
+        <v>7</v>
+      </c>
+      <c r="B16" s="10">
+        <v>1</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
+      <c r="A17" s="10">
+        <v>8</v>
+      </c>
+      <c r="B17" s="10">
+        <v>1</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
+      <c r="A18" s="10">
+        <v>9</v>
+      </c>
+      <c r="B18" s="10">
+        <v>3</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
+      <c r="A19" s="10">
+        <v>10</v>
+      </c>
+      <c r="B19" s="10">
+        <v>3</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
+      <c r="A20" s="10">
+        <v>11</v>
+      </c>
+      <c r="B20" s="10">
+        <v>1</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
+      <c r="A21" s="30">
+        <v>12</v>
+      </c>
+      <c r="B21" s="30">
+        <v>2</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
+      <c r="A22" s="30">
+        <v>13</v>
+      </c>
+      <c r="B22" s="30">
+        <v>1</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
+      <c r="A23" s="10">
+        <v>14</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
+      <c r="A24" s="10">
+        <v>15</v>
+      </c>
+      <c r="B24" s="10">
+        <v>1</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25"/>
+      <c r="A25" s="10">
+        <v>16</v>
+      </c>
+      <c r="B25" s="10">
+        <v>4</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26"/>
+      <c r="A26" s="29">
+        <v>17</v>
+      </c>
+      <c r="B26" s="29">
+        <v>4</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="G27"/>
-      <c r="H27"/>
-      <c r="I27"/>
+      <c r="A27" s="29">
+        <v>18</v>
+      </c>
+      <c r="B27" s="29">
+        <v>2</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
+      <c r="A28" s="10">
+        <v>19</v>
+      </c>
+      <c r="B28" s="10">
+        <v>1</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
+      <c r="A29" s="10">
+        <v>20</v>
+      </c>
+      <c r="B29" s="10">
+        <v>2</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30"/>
+      <c r="A30" s="10">
+        <v>21</v>
+      </c>
+      <c r="B30" s="10">
+        <v>2</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
+      <c r="A31" s="10">
+        <v>22</v>
+      </c>
+      <c r="B31" s="10">
+        <v>1</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
+      <c r="A32" s="10">
+        <v>23</v>
+      </c>
+      <c r="B32" s="10">
+        <v>1</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
+      <c r="A33" s="26">
+        <v>24</v>
+      </c>
+      <c r="B33" s="26">
+        <v>8</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35"/>
+      <c r="A35" s="10">
+        <v>25</v>
+      </c>
+      <c r="B35" s="10">
+        <v>4</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A36"/>
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="F36"/>
-      <c r="G36"/>
-      <c r="H36"/>
-      <c r="I36"/>
+      <c r="A36" s="26">
+        <v>26</v>
+      </c>
+      <c r="B36" s="26">
+        <v>7</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="D36" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38"/>
-      <c r="I38"/>
+      <c r="A38" s="10">
+        <v>27</v>
+      </c>
+      <c r="B38" s="10">
+        <v>1</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39"/>
-      <c r="I39"/>
+      <c r="A39" s="10">
+        <v>28</v>
+      </c>
+      <c r="B39" s="10">
+        <v>1</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40"/>
+      <c r="A40" s="10">
+        <v>29</v>
+      </c>
+      <c r="B40" s="10">
+        <v>1</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-      <c r="G41"/>
-      <c r="H41"/>
-      <c r="I41"/>
+      <c r="A41" s="10">
+        <v>30</v>
+      </c>
+      <c r="B41" s="10">
+        <v>1</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A42"/>
-      <c r="B42"/>
-      <c r="C42"/>
-      <c r="D42"/>
-      <c r="E42"/>
-      <c r="F42"/>
-      <c r="G42"/>
-      <c r="H42"/>
-      <c r="I42"/>
+      <c r="A42" s="10">
+        <v>31</v>
+      </c>
+      <c r="B42" s="10">
+        <v>4</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A43"/>
-      <c r="B43"/>
-      <c r="C43"/>
-      <c r="D43"/>
-      <c r="E43"/>
-      <c r="F43"/>
-      <c r="G43"/>
-      <c r="H43"/>
-      <c r="I43"/>
+      <c r="A43" s="29">
+        <v>32</v>
+      </c>
+      <c r="B43" s="29">
+        <v>2</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="G43" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A44"/>
-      <c r="B44"/>
-      <c r="C44"/>
-      <c r="D44"/>
-      <c r="E44"/>
-      <c r="F44"/>
-      <c r="G44"/>
-      <c r="H44"/>
-      <c r="I44"/>
+      <c r="A44" s="10">
+        <v>33</v>
+      </c>
+      <c r="B44" s="10">
+        <v>5</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A45"/>
-      <c r="B45"/>
-      <c r="C45"/>
-      <c r="D45"/>
-      <c r="E45"/>
-      <c r="F45"/>
-      <c r="G45"/>
-      <c r="H45"/>
-      <c r="I45"/>
+      <c r="A45" s="10">
+        <v>34</v>
+      </c>
+      <c r="B45" s="10">
+        <v>3</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A46"/>
-      <c r="B46"/>
-      <c r="C46"/>
-      <c r="D46"/>
-      <c r="E46"/>
-      <c r="F46"/>
-      <c r="G46"/>
-      <c r="H46"/>
-      <c r="I46"/>
+      <c r="A46" s="10">
+        <v>35</v>
+      </c>
+      <c r="B46" s="10">
+        <v>1</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A47"/>
-      <c r="B47"/>
-      <c r="C47"/>
-      <c r="D47"/>
-      <c r="E47"/>
-      <c r="F47"/>
-      <c r="G47"/>
-      <c r="H47"/>
-      <c r="I47"/>
+      <c r="A47" s="10">
+        <v>36</v>
+      </c>
+      <c r="B47" s="10">
+        <v>1</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A48"/>
-      <c r="B48"/>
-      <c r="C48"/>
-      <c r="D48"/>
-      <c r="E48"/>
-      <c r="F48"/>
-      <c r="G48"/>
-      <c r="H48"/>
-      <c r="I48"/>
+      <c r="A48" s="10">
+        <v>37</v>
+      </c>
+      <c r="B48" s="10">
+        <v>4</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A49"/>
-      <c r="B49"/>
-      <c r="C49"/>
-      <c r="D49"/>
-      <c r="E49"/>
-      <c r="F49"/>
-      <c r="G49"/>
-      <c r="H49"/>
-      <c r="I49"/>
+      <c r="A49" s="10">
+        <v>38</v>
+      </c>
+      <c r="B49" s="10">
+        <v>1</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A50"/>
-      <c r="B50"/>
-      <c r="C50"/>
-      <c r="D50"/>
-      <c r="E50"/>
-      <c r="F50"/>
-      <c r="G50"/>
-      <c r="H50"/>
-      <c r="I50"/>
+      <c r="A50" s="10">
+        <v>39</v>
+      </c>
+      <c r="B50" s="10">
+        <v>1</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A51"/>
-      <c r="B51"/>
-      <c r="C51"/>
-      <c r="D51"/>
-      <c r="E51"/>
-      <c r="F51"/>
-      <c r="G51"/>
-      <c r="H51"/>
-      <c r="I51"/>
+      <c r="A51" s="10">
+        <v>40</v>
+      </c>
+      <c r="B51" s="10">
+        <v>1</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A52"/>
-      <c r="B52"/>
-      <c r="C52"/>
-      <c r="D52"/>
-      <c r="E52"/>
-      <c r="F52"/>
-      <c r="G52"/>
-      <c r="H52"/>
-      <c r="I52"/>
+      <c r="A52" s="10">
+        <v>41</v>
+      </c>
+      <c r="B52" s="10">
+        <v>1</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A53"/>
-      <c r="B53"/>
-      <c r="C53"/>
-      <c r="D53"/>
-      <c r="E53"/>
-      <c r="F53"/>
-      <c r="G53"/>
-      <c r="H53"/>
-      <c r="I53"/>
+      <c r="A53" s="10">
+        <v>42</v>
+      </c>
+      <c r="B53" s="10">
+        <v>1</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A54"/>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="D54"/>
-      <c r="E54"/>
-      <c r="F54"/>
-      <c r="G54"/>
-      <c r="H54"/>
-      <c r="I54"/>
+      <c r="A54" s="10">
+        <v>43</v>
+      </c>
+      <c r="B54" s="10">
+        <v>1</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A55"/>
-      <c r="B55"/>
-      <c r="C55"/>
-      <c r="D55"/>
-      <c r="E55"/>
-      <c r="F55"/>
-      <c r="G55"/>
-      <c r="H55"/>
-      <c r="I55"/>
+      <c r="A55" s="10">
+        <v>44</v>
+      </c>
+      <c r="B55" s="10">
+        <v>1</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A56"/>
-      <c r="B56"/>
-      <c r="C56"/>
-      <c r="D56"/>
-      <c r="E56"/>
-      <c r="F56"/>
-      <c r="G56"/>
-      <c r="H56"/>
-      <c r="I56"/>
+      <c r="A56" s="10">
+        <v>45</v>
+      </c>
+      <c r="B56" s="10">
+        <v>1</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A57"/>
-      <c r="B57"/>
-      <c r="C57"/>
-      <c r="D57"/>
-      <c r="E57"/>
-      <c r="F57"/>
-      <c r="G57"/>
-      <c r="H57"/>
-      <c r="I57"/>
+      <c r="A57" s="10">
+        <v>46</v>
+      </c>
+      <c r="B57" s="10">
+        <v>1</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A58"/>
-      <c r="B58"/>
-      <c r="C58"/>
-      <c r="D58"/>
-      <c r="E58"/>
-      <c r="F58"/>
-      <c r="G58"/>
-      <c r="H58"/>
-      <c r="I58"/>
+      <c r="A58" s="10">
+        <v>47</v>
+      </c>
+      <c r="B58" s="10">
+        <v>1</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A59"/>
-      <c r="B59"/>
-      <c r="C59"/>
-      <c r="D59"/>
-      <c r="E59"/>
-      <c r="F59"/>
-      <c r="G59"/>
-      <c r="H59"/>
-      <c r="I59"/>
+      <c r="A59" s="10">
+        <v>48</v>
+      </c>
+      <c r="B59" s="10">
+        <v>1</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A60"/>
-      <c r="B60"/>
-      <c r="C60"/>
-      <c r="D60"/>
-      <c r="E60"/>
-      <c r="F60"/>
-      <c r="G60"/>
-      <c r="H60"/>
-      <c r="I60"/>
+      <c r="A60" s="10">
+        <v>49</v>
+      </c>
+      <c r="B60" s="10">
+        <v>1</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A61"/>
-      <c r="B61"/>
-      <c r="C61"/>
-      <c r="D61"/>
-      <c r="E61"/>
-      <c r="F61"/>
-      <c r="G61"/>
-      <c r="H61"/>
-      <c r="I61"/>
+      <c r="A61" s="10">
+        <v>50</v>
+      </c>
+      <c r="B61" s="10">
+        <v>1</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A62"/>
-      <c r="B62"/>
-      <c r="C62"/>
-      <c r="D62"/>
-      <c r="E62"/>
-      <c r="F62"/>
-      <c r="G62"/>
-      <c r="H62"/>
-      <c r="I62"/>
+      <c r="A62" s="10">
+        <v>51</v>
+      </c>
+      <c r="B62" s="10">
+        <v>1</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A63"/>
-      <c r="B63"/>
-      <c r="C63"/>
-      <c r="D63"/>
-      <c r="E63"/>
-      <c r="F63"/>
-      <c r="G63"/>
-      <c r="H63"/>
-      <c r="I63"/>
+      <c r="A63" s="10">
+        <v>52</v>
+      </c>
+      <c r="B63" s="10">
+        <v>2</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A64"/>
-      <c r="B64"/>
-      <c r="C64"/>
-      <c r="D64"/>
-      <c r="E64"/>
-      <c r="F64"/>
-      <c r="G64"/>
-      <c r="H64"/>
-      <c r="I64"/>
+      <c r="A64" s="10">
+        <v>53</v>
+      </c>
+      <c r="B64" s="10">
+        <v>1</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A65"/>
-      <c r="B65"/>
-      <c r="C65"/>
-      <c r="D65"/>
-      <c r="E65"/>
-      <c r="F65"/>
-      <c r="G65"/>
-      <c r="H65"/>
-      <c r="I65"/>
+      <c r="A65" s="10">
+        <v>54</v>
+      </c>
+      <c r="B65" s="10">
+        <v>1</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A66"/>
-      <c r="B66"/>
-      <c r="C66"/>
-      <c r="D66"/>
-      <c r="E66"/>
-      <c r="F66"/>
-      <c r="G66"/>
-      <c r="H66"/>
-      <c r="I66"/>
+      <c r="A66" s="9"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A67"/>
-      <c r="B67"/>
-      <c r="C67"/>
-      <c r="D67"/>
-      <c r="E67"/>
-      <c r="F67"/>
-      <c r="G67"/>
-      <c r="H67"/>
-      <c r="I67"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A68"/>

</xml_diff>